<commit_message>
Bug fix in carbon cycle model, forest carbon sequestration is now accounted for.
</commit_message>
<xml_diff>
--- a/RECC_ModelConfig_List_V2_4.xlsx
+++ b/RECC_ModelConfig_List_V2_4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RECC_Config_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9045" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9189" uniqueCount="365">
   <si>
     <t>Sheet_Name</t>
   </si>
@@ -766,6 +766,360 @@
   </si>
   <si>
     <t>[33]</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_41_25_reb_</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_50_27_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_52_2_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_53_37_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_55_13_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_56_49_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_58_27_pav_</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__22_59_59_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__23_1_31_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__23_3_2_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__23_4_33_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__23_6_4_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>Poland_2020_6_20__23_7_35_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_9_6_reb_</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_18_26_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_20_3_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_21_41_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_23_20_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_25_0_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_26_40_pav_</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_28_13_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_29_45_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_31_17_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_32_50_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_34_22_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R32JPN_2020_6_20__23_35_54_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_37_31_reb_</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_46_57_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_48_39_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_50_21_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_52_3_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_53_45_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_55_27_pav_</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_57_1_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_20__23_58_35_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_21__0_0_9_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_21__0_1_44_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_21__0_3_18_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R32CHN_2020_6_21__0_4_52_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_6_26_reb_</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_15_51_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_17_33_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_19_15_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_20_57_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_22_38_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_24_20_reb_</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_26_2_reb__FYI</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_27_44_reb__FSD</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_29_26_reb__EoL</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_31_9_reb__MSU</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_32_52_reb__ULD</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_34_34_reb__RUS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_36_16_reb__LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_37_58_reb__MIU</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_39_41_reb__NoR</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_41_22_pav_</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_42_57_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_44_31_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_46_5_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_47_39_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_49_13_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_50_46_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_52_21_pav_</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_53_55_pav__FYI</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_55_29_pav__FSD</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_57_3_pav__EoL</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__0_58_36_pav__MSU</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_0_10_pav__ULD</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_1_44_pav__RUS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_3_17_pav__LTE</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_4_51_pav__CaS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_6_25_pav__RiS</t>
+  </si>
+  <si>
+    <t>R32IND_2020_6_21__1_7_59_pav__NoR</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_9_33_reb_</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_18_59_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_20_41_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_22_23_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_24_5_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_25_47_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_27_28_pav_</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_29_2_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_30_37_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_32_11_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_33_44_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_35_18_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other_2020_6_21__1_36_52_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_38_25_reb_</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_47_51_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_49_32_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_51_12_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_52_53_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_54_34_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_56_15_pav_</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_57_48_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__1_59_21_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__2_0_53_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__2_2_26_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__2_3_59_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other_2020_6_21__2_5_32_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_7_5_reb_</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_16_27_reb__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_18_8_reb__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_19_49_reb__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_21_30_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_23_10_reb__FYI_FSD_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_24_51_pav_</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_26_24_pav__FYI_FSD_EoL</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_27_57_pav__FYI_FSD_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_29_29_pav__FYI_FSD_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_31_2_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_32_36_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS</t>
+  </si>
+  <si>
+    <t>R5.2SSA_Other_2020_6_21__2_34_9_pav__FYI_FSD_EoL_MSU_ULD_RUS_LTE_CaS_RiS</t>
+  </si>
+  <si>
+    <t>OECD_Other</t>
+  </si>
+  <si>
+    <t>ASIA_Other</t>
+  </si>
+  <si>
+    <t>SSA_Other</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -1125,11 +1479,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:Y115"/>
+      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28780,10 +29134,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D91"/>
+  <dimension ref="B1:D203"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29319,6 +29673,662 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" t="s">
+        <v>43</v>
+      </c>
+      <c r="D91" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D92" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D94" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D95" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D96" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B97" t="s">
+        <v>234</v>
+      </c>
+      <c r="C97" t="s">
+        <v>100</v>
+      </c>
+      <c r="D97" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D98" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D99" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D100" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D101" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D102" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D103" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B104" t="s">
+        <v>362</v>
+      </c>
+      <c r="C104" t="s">
+        <v>43</v>
+      </c>
+      <c r="D104" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D105" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D106" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D107" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D108" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D109" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B110" t="s">
+        <v>362</v>
+      </c>
+      <c r="C110" t="s">
+        <v>100</v>
+      </c>
+      <c r="D110" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D111" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D112" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D114" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D115" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D116" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B117" t="s">
+        <v>363</v>
+      </c>
+      <c r="C117" t="s">
+        <v>43</v>
+      </c>
+      <c r="D117" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D118" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D119" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D120" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D121" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D122" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B123" t="s">
+        <v>363</v>
+      </c>
+      <c r="C123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D123" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D124" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D125" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D126" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D127" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D128" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D129" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B130" t="s">
+        <v>364</v>
+      </c>
+      <c r="C130" t="s">
+        <v>43</v>
+      </c>
+      <c r="D130" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D131" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D132" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D133" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D134" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D135" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B136" t="s">
+        <v>364</v>
+      </c>
+      <c r="C136" t="s">
+        <v>173</v>
+      </c>
+      <c r="D136" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D137" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D138" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D139" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D140" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D141" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D142" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D143" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D144" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D145" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B146" t="s">
+        <v>364</v>
+      </c>
+      <c r="C146" t="s">
+        <v>100</v>
+      </c>
+      <c r="D146" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D147" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D148" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D149" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D150" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D151" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D152" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B153" t="s">
+        <v>364</v>
+      </c>
+      <c r="C153" t="s">
+        <v>172</v>
+      </c>
+      <c r="D153" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D154" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D155" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D156" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D157" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D158" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D159" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D160" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D161" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D162" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D163" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B164" t="s">
+        <v>359</v>
+      </c>
+      <c r="C164" t="s">
+        <v>43</v>
+      </c>
+      <c r="D164" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D165" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D166" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D167" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D168" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D169" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B170" t="s">
+        <v>359</v>
+      </c>
+      <c r="C170" t="s">
+        <v>100</v>
+      </c>
+      <c r="D170" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D171" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D172" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D173" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D174" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D175" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D176" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B177" t="s">
+        <v>360</v>
+      </c>
+      <c r="C177" t="s">
+        <v>43</v>
+      </c>
+      <c r="D177" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D178" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D179" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D180" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D181" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D182" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B183" t="s">
+        <v>360</v>
+      </c>
+      <c r="C183" t="s">
+        <v>100</v>
+      </c>
+      <c r="D183" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D184" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D185" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D186" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D187" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D188" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D189" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B190" t="s">
+        <v>361</v>
+      </c>
+      <c r="C190" t="s">
+        <v>43</v>
+      </c>
+      <c r="D190" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D191" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D192" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D193" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D194" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D195" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B196" t="s">
+        <v>361</v>
+      </c>
+      <c r="C196" t="s">
+        <v>100</v>
+      </c>
+      <c r="D196" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D197" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D198" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D199" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D200" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D201" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D202" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B203" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final changes to figures and data export for v2.4 (GLOBAL) version.
</commit_message>
<xml_diff>
--- a/RECC_ModelConfig_List_V2_4.xlsx
+++ b/RECC_ModelConfig_List_V2_4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pav_reb_Config_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14285" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14302" uniqueCount="724">
   <si>
     <t>Group</t>
   </si>
@@ -2608,7 +2608,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -41465,16 +41465,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M426"/>
+  <dimension ref="A1:M426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="19.86328125" customWidth="1"/>
-    <col min="3" max="3" width="28.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.265625" customWidth="1"/>
     <col min="4" max="4" width="77.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.265625" customWidth="1"/>
     <col min="6" max="6" width="25.59765625" bestFit="1" customWidth="1"/>
@@ -41654,13 +41654,13 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>307</v>
+        <v>42</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>513</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -41670,11 +41670,9 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" t="s">
-        <v>308</v>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D17" s="10" t="s">
+        <v>514</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -41684,11 +41682,9 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" t="s">
-        <v>309</v>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D18" s="10" t="s">
+        <v>515</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -41698,11 +41694,9 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" t="s">
-        <v>310</v>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D19" s="10" t="s">
+        <v>516</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -41712,11 +41706,9 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" t="s">
-        <v>311</v>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D20" s="10" t="s">
+        <v>517</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -41726,11 +41718,9 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" t="s">
-        <v>312</v>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D21" s="10" t="s">
+        <v>518</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -41740,11 +41730,15 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" t="s">
-        <v>313</v>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>519</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -41756,11 +41750,9 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" t="s">
-        <v>314</v>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D23" s="10" t="s">
+        <v>520</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -41772,15 +41764,9 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D24" t="s">
-        <v>712</v>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D24" s="10" t="s">
+        <v>521</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -41792,15 +41778,9 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D25" t="s">
-        <v>713</v>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D25" s="10" t="s">
+        <v>522</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -41812,15 +41792,9 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D26" t="s">
-        <v>714</v>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D26" s="10" t="s">
+        <v>523</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -41832,15 +41806,9 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D27" t="s">
-        <v>715</v>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D27" s="10" t="s">
+        <v>524</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -41852,15 +41820,9 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>184</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D28" t="s">
-        <v>716</v>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D28" s="10" t="s">
+        <v>525</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -41872,15 +41834,16 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="8"/>
       <c r="B29" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>281</v>
+      <c r="C29" t="s">
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>717</v>
+        <v>307</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -41892,15 +41855,11 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B30" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>643</v>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" t="s">
+        <v>308</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -41912,11 +41871,11 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="10" t="s">
-        <v>644</v>
+      <c r="D31" t="s">
+        <v>309</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -41928,11 +41887,11 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="10" t="s">
-        <v>645</v>
+      <c r="D32" t="s">
+        <v>310</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -41947,8 +41906,8 @@
     <row r="33" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="10" t="s">
-        <v>646</v>
+      <c r="D33" t="s">
+        <v>311</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -41963,8 +41922,8 @@
     <row r="34" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="10" t="s">
-        <v>647</v>
+      <c r="D34" t="s">
+        <v>312</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -41979,8 +41938,8 @@
     <row r="35" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="10" t="s">
-        <v>648</v>
+      <c r="D35" t="s">
+        <v>313</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -41995,114 +41954,224 @@
     <row r="36" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="10" t="s">
-        <v>649</v>
+      <c r="D36" t="s">
+        <v>314</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="10" t="s">
-        <v>650</v>
+      <c r="B37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D37" t="s">
+        <v>712</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>718</v>
+      <c r="D38" t="s">
+        <v>713</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>719</v>
+      <c r="D39" t="s">
+        <v>714</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>720</v>
+      <c r="D40" t="s">
+        <v>715</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>721</v>
+      <c r="D41" t="s">
+        <v>716</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>722</v>
+      <c r="D42" t="s">
+        <v>717</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B43" t="s">
+      <c r="B43" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>281</v>
+      <c r="C43" t="s">
+        <v>60</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>723</v>
+        <v>643</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="10" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="10" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="10" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="10" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="10" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="10" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B57" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="D45" s="10"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="D48" s="10"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D77" s="10"/>
@@ -42449,8 +42518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H445"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B439" sqref="B439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -45704,8 +45773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -46107,8 +46176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:S32"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Changed final paper color codings and added IIASA database export routine.
</commit_message>
<xml_diff>
--- a/RECC_ModelConfig_List_V2_4.xlsx
+++ b/RECC_ModelConfig_List_V2_4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pav_reb_Config_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14302" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14285" uniqueCount="724">
   <si>
     <t>Group</t>
   </si>
@@ -41465,10 +41465,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M426"/>
+  <dimension ref="A1:M413"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -41480,7 +41480,7 @@
     <col min="6" max="6" width="25.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
@@ -41491,7 +41491,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>63</v>
       </c>
@@ -41502,37 +41502,37 @@
         <v>698</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>705</v>
       </c>
@@ -41544,7 +41544,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
         <v>63</v>
       </c>
@@ -41562,7 +41562,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>63</v>
       </c>
@@ -41580,7 +41580,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
         <v>63</v>
       </c>
@@ -41598,7 +41598,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>63</v>
       </c>
@@ -41616,7 +41616,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
         <v>63</v>
       </c>
@@ -41634,7 +41634,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
         <v>63</v>
       </c>
@@ -41652,16 +41652,19 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="8"/>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>513</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -41670,10 +41673,14 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D17" s="10" t="s">
-        <v>514</v>
-      </c>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -41682,10 +41689,14 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D18" s="10" t="s">
-        <v>515</v>
-      </c>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" t="s">
+        <v>309</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -41694,10 +41705,14 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D19" s="10" t="s">
-        <v>516</v>
-      </c>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" t="s">
+        <v>310</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -41706,10 +41721,14 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D20" s="10" t="s">
-        <v>517</v>
-      </c>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" t="s">
+        <v>311</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -41718,10 +41737,14 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D21" s="10" t="s">
-        <v>518</v>
-      </c>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" t="s">
+        <v>312</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -41730,15 +41753,11 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>519</v>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" t="s">
+        <v>313</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -41750,428 +41769,266 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D23" s="10" t="s">
-        <v>520</v>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" t="s">
+        <v>314</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D24" s="10" t="s">
-        <v>521</v>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" t="s">
+        <v>712</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D25" s="10" t="s">
-        <v>522</v>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" t="s">
+        <v>713</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D26" s="10" t="s">
-        <v>523</v>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" t="s">
+        <v>714</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D27" s="10" t="s">
-        <v>524</v>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" t="s">
+        <v>715</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="D28" s="10" t="s">
-        <v>525</v>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D28" t="s">
+        <v>716</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="8"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>184</v>
       </c>
-      <c r="C29" t="s">
-        <v>60</v>
+      <c r="C29" s="8" t="s">
+        <v>281</v>
       </c>
       <c r="D29" t="s">
-        <v>307</v>
+        <v>717</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" t="s">
-        <v>308</v>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B30" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>643</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" t="s">
-        <v>309</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="D31" s="10" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" t="s">
-        <v>310</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D32" s="10" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" t="s">
-        <v>311</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D33" s="10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" t="s">
-        <v>312</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D34" s="10" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" t="s">
-        <v>313</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D35" s="10" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" t="s">
-        <v>314</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>184</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D37" t="s">
-        <v>712</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D36" s="10" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="10" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D38" t="s">
-        <v>713</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D38" s="10" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D39" t="s">
-        <v>714</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D39" s="10" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D40" t="s">
-        <v>715</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D40" s="10" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D41" t="s">
-        <v>716</v>
-      </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D41" s="10" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D42" t="s">
-        <v>717</v>
-      </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B43" s="8" t="s">
+      <c r="D42" s="10" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
         <v>185</v>
       </c>
-      <c r="C43" t="s">
-        <v>60</v>
+      <c r="C43" s="8" t="s">
+        <v>281</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B44" s="8"/>
+        <v>723</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B44" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="C44" s="8"/>
-      <c r="D44" s="10" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="10" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="10" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="10" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="10" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="10" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="10" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B51" t="s">
-        <v>185</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B52" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B53" t="s">
-        <v>185</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B55" t="s">
-        <v>185</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B56" t="s">
-        <v>185</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D77" s="10"/>
@@ -42233,44 +42090,42 @@
     <row r="96" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D97" s="10"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D98" s="10"/>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D99" s="10"/>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D100" s="10"/>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D101" s="10"/>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D102" s="10"/>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D103" s="10"/>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D104" s="10"/>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D105" s="10"/>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D106" s="10"/>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D107" s="10"/>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D108" s="10"/>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D109" s="10"/>
+    <row r="359" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B359" s="8"/>
+      <c r="C359" s="8"/>
+      <c r="D359" s="8"/>
+    </row>
+    <row r="360" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B360" s="8"/>
+      <c r="C360" s="8"/>
+      <c r="D360" s="8"/>
+    </row>
+    <row r="361" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B361" s="8"/>
+      <c r="C361" s="8"/>
+      <c r="D361" s="8"/>
+    </row>
+    <row r="362" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B362" s="8"/>
+      <c r="C362" s="8"/>
+      <c r="D362" s="8"/>
+    </row>
+    <row r="368" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B368" s="8"/>
+      <c r="D368" s="8"/>
+    </row>
+    <row r="369" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D369" s="8"/>
+    </row>
+    <row r="370" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B370" s="8"/>
+      <c r="C370" s="8"/>
+      <c r="D370" s="8"/>
+    </row>
+    <row r="371" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B371" s="8"/>
+      <c r="C371" s="8"/>
+      <c r="D371" s="8"/>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B372" s="8"/>
@@ -42292,11 +42147,39 @@
       <c r="C375" s="8"/>
       <c r="D375" s="8"/>
     </row>
+    <row r="376" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B376" s="8"/>
+      <c r="C376" s="8"/>
+      <c r="D376" s="8"/>
+    </row>
+    <row r="377" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B377" s="8"/>
+      <c r="C377" s="8"/>
+      <c r="D377" s="8"/>
+    </row>
+    <row r="378" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B378" s="8"/>
+      <c r="C378" s="8"/>
+      <c r="D378" s="8"/>
+    </row>
+    <row r="379" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B379" s="8"/>
+      <c r="C379" s="8"/>
+      <c r="D379" s="8"/>
+    </row>
+    <row r="380" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B380" s="8"/>
+      <c r="C380" s="8"/>
+      <c r="D380" s="8"/>
+    </row>
     <row r="381" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B381" s="8"/>
+      <c r="C381" s="8"/>
       <c r="D381" s="8"/>
     </row>
     <row r="382" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B382" s="8"/>
+      <c r="C382" s="8"/>
       <c r="D382" s="8"/>
     </row>
     <row r="383" spans="2:4" x14ac:dyDescent="0.45">
@@ -42330,71 +42213,66 @@
       <c r="D388" s="8"/>
     </row>
     <row r="389" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B389" s="8"/>
-      <c r="C389" s="8"/>
-      <c r="D389" s="8"/>
+      <c r="D389" s="9"/>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B390" s="8"/>
       <c r="C390" s="8"/>
-      <c r="D390" s="8"/>
+      <c r="D390" s="9"/>
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B391" s="8"/>
       <c r="C391" s="8"/>
-      <c r="D391" s="8"/>
+      <c r="D391" s="9"/>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B392" s="8"/>
       <c r="C392" s="8"/>
-      <c r="D392" s="8"/>
+      <c r="D392" s="9"/>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B393" s="8"/>
       <c r="C393" s="8"/>
-      <c r="D393" s="8"/>
+      <c r="D393" s="9"/>
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B394" s="8"/>
       <c r="C394" s="8"/>
-      <c r="D394" s="8"/>
+      <c r="D394" s="9"/>
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B395" s="8"/>
       <c r="C395" s="8"/>
-      <c r="D395" s="8"/>
+      <c r="D395" s="9"/>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B396" s="8"/>
       <c r="C396" s="8"/>
-      <c r="D396" s="8"/>
+      <c r="D396" s="9"/>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B397" s="8"/>
       <c r="C397" s="8"/>
-      <c r="D397" s="8"/>
+      <c r="D397" s="9"/>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B398" s="8"/>
       <c r="C398" s="8"/>
-      <c r="D398" s="8"/>
+      <c r="D398" s="9"/>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B399" s="8"/>
       <c r="C399" s="8"/>
-      <c r="D399" s="8"/>
+      <c r="D399" s="9"/>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B400" s="8"/>
       <c r="C400" s="8"/>
-      <c r="D400" s="8"/>
+      <c r="D400" s="9"/>
     </row>
     <row r="401" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B401" s="8"/>
-      <c r="C401" s="8"/>
-      <c r="D401" s="8"/>
+      <c r="D401" s="9"/>
     </row>
     <row r="402" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B402" s="8"/>
+      <c r="C402" s="8"/>
       <c r="D402" s="9"/>
     </row>
     <row r="403" spans="2:4" x14ac:dyDescent="0.45">
@@ -42428,7 +42306,6 @@
       <c r="D408" s="9"/>
     </row>
     <row r="409" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B409" s="8"/>
       <c r="C409" s="8"/>
       <c r="D409" s="9"/>
     </row>
@@ -42445,68 +42322,9 @@
       <c r="D412" s="9"/>
     </row>
     <row r="413" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B413" s="8"/>
       <c r="C413" s="8"/>
-      <c r="D413" s="9"/>
-    </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B414" s="8"/>
-      <c r="D414" s="9"/>
-    </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B415" s="8"/>
-      <c r="C415" s="8"/>
-      <c r="D415" s="9"/>
-    </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B416" s="8"/>
-      <c r="C416" s="8"/>
-      <c r="D416" s="9"/>
-    </row>
-    <row r="417" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B417" s="8"/>
-      <c r="C417" s="8"/>
-      <c r="D417" s="9"/>
-    </row>
-    <row r="418" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B418" s="8"/>
-      <c r="C418" s="8"/>
-      <c r="D418" s="9"/>
-    </row>
-    <row r="419" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B419" s="8"/>
-      <c r="C419" s="8"/>
-      <c r="D419" s="9"/>
-    </row>
-    <row r="420" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B420" s="8"/>
-      <c r="C420" s="8"/>
-      <c r="D420" s="9"/>
-    </row>
-    <row r="421" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B421" s="8"/>
-      <c r="C421" s="8"/>
-      <c r="D421" s="9"/>
-    </row>
-    <row r="422" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C422" s="8"/>
-      <c r="D422" s="9"/>
-    </row>
-    <row r="423" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C423" s="8"/>
-      <c r="D423" s="9"/>
-    </row>
-    <row r="424" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C424" s="8"/>
-      <c r="D424" s="9"/>
-    </row>
-    <row r="425" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C425" s="8"/>
-      <c r="D425" s="9"/>
-    </row>
-    <row r="426" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B426" s="8"/>
-      <c r="C426" s="8"/>
-      <c r="D426" s="8"/>
+      <c r="D413" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -42518,7 +42336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H445"/>
   <sheetViews>
-    <sheetView topLeftCell="A390" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B439" sqref="B439"/>
     </sheetView>
   </sheetViews>
@@ -45773,7 +45591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>

</xml_diff>